<commit_message>
automação selenium em execução
</commit_message>
<xml_diff>
--- a/operadoras_sem_arquivos_hoje.xlsx
+++ b/operadoras_sem_arquivos_hoje.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BENVISAVALE</t>
+          <t>BMGCARD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BMGCARD</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>BOLETOBB</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BOLETOBB</t>
+          <t>BRASILCARDNET</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BRASILCARDNET</t>
+          <t>BRASILCONVENIOS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BRASILCONVENIOS</t>
+          <t>CABOSESOLDADOS</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CABOSESOLDADOS</t>
+          <t>CALCARD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CALCARD</t>
+          <t>CARTAOPREDATADO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CARTAOPREDATADO</t>
+          <t>CETELEM</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CETELEM</t>
+          <t>CONVENIOSCARD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CONVENIOSCARD</t>
+          <t>CREDNOSSO</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CREDNOSSO</t>
+          <t>CREDZ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CREDZ</t>
+          <t>CROSCARD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CROSCARD</t>
+          <t>CSF</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CSF</t>
+          <t>DESCONHECIDO</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DESCONHECIDO</t>
+          <t>DIGIMODAS</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DIGIMODAS</t>
+          <t>ELAVON</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ELAVON</t>
+          <t>GLOBAL PAYMENTS</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GLOBAL PAYMENTS</t>
+          <t>GREENCARD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GREENCARD</t>
+          <t>HELLOTICKET</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HELLOTICKET</t>
+          <t>INOVEPAY</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>INOVEPAY</t>
+          <t>ITI</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ITI</t>
+          <t>KOIN</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>KOIN</t>
+          <t>LAGOACRED</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LAGOACRED</t>
+          <t>LINXPAY</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LINXPAY</t>
+          <t>LOSANGO</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LOSANGO</t>
+          <t>MAISFACIL</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MAISFACIL</t>
+          <t>MAXI CARTÃO</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MAXI CARTÃO</t>
+          <t>OPERADORA TESTE CODIGO</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>OPERADORA TESTE CODIGO</t>
+          <t>PAGOLIVRE</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PAGOLIVRE</t>
+          <t>PAGSIMPLES</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -856,7 +856,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PAGSIMPLES</t>
+          <t>PAGUELOGO</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PAGUELOGO</t>
+          <t>PEDEPRONTO</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PEDEPRONTO</t>
+          <t>PITCARD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PITCARD</t>
+          <t>PIXBB</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PIXBB</t>
+          <t>RAPPI</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>RAPPI</t>
+          <t>REDEMED</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>RAPPI FARMACIA</t>
+          <t>REDETREL</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>REDEMED</t>
+          <t>SESIMAX</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>REDETREL</t>
+          <t>SICREDI</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SESIMAX</t>
+          <t>SINDPLUS</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SICREDI</t>
+          <t>SOLUCARD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -988,7 +988,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SINDPLUS</t>
+          <t>SOMA CONTA DIGITAL</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>SOLUCARD</t>
+          <t>SOROCRED</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>SOMA CONTA DIGITAL</t>
+          <t>TEGYNBTEN</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>SOROCRED</t>
+          <t>TESTE</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1036,7 +1036,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TEGYNBTEN</t>
+          <t>TESTE</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>TESTE32</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>TICKET</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1072,7 +1072,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TESTE32</t>
+          <t>TODOCARTOES</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TICKET</t>
+          <t>UBEREATS</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>TODOCARTOES</t>
+          <t>USACARD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>UBEREATS</t>
+          <t>VALECON</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>USACARD</t>
+          <t>VALEMAIS</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1132,46 +1132,10 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>VALECON</t>
+          <t>WEBCARD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
-        <is>
-          <t>13/05/25</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>VALEMAIS</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>13/05/25</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>WEBCARD</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>13/05/25</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>WIZEO</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
         <is>
           <t>13/05/25</t>
         </is>

</xml_diff>